<commit_message>
start time position change in catch basin and ows forms
</commit_message>
<xml_diff>
--- a/app/config/tables/catchBasinInspectionForm/forms/catchBasinInspectionForm/catchBasinInspectionForm.xlsx
+++ b/app/config/tables/catchBasinInspectionForm/forms/catchBasinInspectionForm/catchBasinInspectionForm.xlsx
@@ -16,11 +16,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="309">
+  <si>
+    <t>query_name</t>
+  </si>
+  <si>
+    <t>branch_label</t>
+  </si>
   <si>
     <t>clause</t>
   </si>
   <si>
+    <t>query_type</t>
+  </si>
+  <si>
+    <t>uri</t>
+  </si>
+  <si>
+    <t>callback</t>
+  </si>
+  <si>
+    <t>linked_form_id</t>
+  </si>
+  <si>
     <t>condition</t>
   </si>
   <si>
@@ -30,24 +48,6 @@
     <t>display.text</t>
   </si>
   <si>
-    <t>query_name</t>
-  </si>
-  <si>
-    <t>branch_label</t>
-  </si>
-  <si>
-    <t>query_type</t>
-  </si>
-  <si>
-    <t>uri</t>
-  </si>
-  <si>
-    <t>callback</t>
-  </si>
-  <si>
-    <t>linked_form_id</t>
-  </si>
-  <si>
     <t>linked_table_id</t>
   </si>
   <si>
@@ -66,16 +66,43 @@
     <t>linked_table</t>
   </si>
   <si>
+    <t>if // start</t>
+  </si>
+  <si>
     <t>catchBasinInspectionSample</t>
   </si>
   <si>
-    <t>if // start</t>
+    <t>(opendatakit.getCurrentInstanceId() != null)</t>
   </si>
   <si>
     <t>global_id = ?</t>
   </si>
   <si>
-    <t>(opendatakit.getCurrentInstanceId() != null)</t>
+    <t>do section survey</t>
+  </si>
+  <si>
+    <t>finalize</t>
+  </si>
+  <si>
+    <t>Save form</t>
+  </si>
+  <si>
+    <t>[ data('global_id') ]</t>
+  </si>
+  <si>
+    <t>else // start</t>
+  </si>
+  <si>
+    <t>'global_id='+encodeURIComponent(data('global_id'))+'&amp;z_sample_date='+encodeURIComponent(data('sample_date'))</t>
+  </si>
+  <si>
+    <t>instances</t>
+  </si>
+  <si>
+    <t>Saved instances</t>
+  </si>
+  <si>
+    <t>end if // start</t>
   </si>
   <si>
     <t>values_list</t>
@@ -87,33 +114,6 @@
     <t>choice_filter</t>
   </si>
   <si>
-    <t>do section survey</t>
-  </si>
-  <si>
-    <t>finalize</t>
-  </si>
-  <si>
-    <t>Save form</t>
-  </si>
-  <si>
-    <t>else // start</t>
-  </si>
-  <si>
-    <t>instances</t>
-  </si>
-  <si>
-    <t>Saved instances</t>
-  </si>
-  <si>
-    <t>[ data('global_id') ]</t>
-  </si>
-  <si>
-    <t>end if // start</t>
-  </si>
-  <si>
-    <t>'global_id='+encodeURIComponent(data('global_id'))+'&amp;z_sample_date='+encodeURIComponent(data('sample_date'))</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -180,30 +180,60 @@
     <t>hidden_input_type.handlebars</t>
   </si>
   <si>
+    <t>choice_list_name</t>
+  </si>
+  <si>
+    <t>data_value</t>
+  </si>
+  <si>
     <t>loc_name</t>
   </si>
   <si>
     <t>opendatakit.getLocationInfo().name</t>
   </si>
   <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>inspection_types</t>
+  </si>
+  <si>
+    <t>Annual Inspection</t>
+  </si>
+  <si>
     <t>loc_aid</t>
   </si>
   <si>
     <t>calculates.locationAid()</t>
   </si>
   <si>
+    <t>Quarterly Inspection</t>
+  </si>
+  <si>
+    <t>Monthly Inspection</t>
+  </si>
+  <si>
+    <t>Re-Inspection</t>
+  </si>
+  <si>
     <t>loc_streetAddress</t>
   </si>
   <si>
     <t>opendatakit.getLocationInfo().streetAddress</t>
   </si>
   <si>
-    <t>choice_list_name</t>
-  </si>
-  <si>
-    <t>data_value</t>
-  </si>
-  <si>
     <t>loc_city</t>
   </si>
   <si>
@@ -216,48 +246,18 @@
     <t>opendatakit.getLocationInfo().state</t>
   </si>
   <si>
-    <t>yesno</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>loc_zip</t>
   </si>
   <si>
     <t>calculates.locationZip()</t>
   </si>
   <si>
-    <t>inspection_types</t>
-  </si>
-  <si>
-    <t>Annual Inspection</t>
-  </si>
-  <si>
-    <t>Quarterly Inspection</t>
-  </si>
-  <si>
     <t>loc_client</t>
   </si>
   <si>
-    <t>Monthly Inspection</t>
-  </si>
-  <si>
     <t>opendatakit.getLocationInfo().client</t>
   </si>
   <si>
-    <t>Re-Inspection</t>
-  </si>
-  <si>
     <t>sample_date</t>
   </si>
   <si>
@@ -585,28 +585,22 @@
     <t>Repair of Defective Part</t>
   </si>
   <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>project_start_time</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>time_input_type.handlebars</t>
+  </si>
+  <si>
     <t>Add Catch Basins to this list</t>
   </si>
   <si>
     <t>Add Catch Basin</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>project_start_time</t>
-  </si>
-  <si>
-    <t>Start Time</t>
-  </si>
-  <si>
-    <t>time_input_type.handlebars</t>
-  </si>
-  <si>
-    <t>project_end_time</t>
-  </si>
-  <si>
-    <t>End Time</t>
   </si>
   <si>
     <t>end screen</t>
@@ -1280,11 +1274,11 @@
       <name val="Arial"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <color rgb="FF444444"/>
+      <name val="'Trebuchet MS'"/>
     </font>
     <font>
-      <color rgb="FF444444"/>
-      <name val="'Trebuchet MS'"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -1330,22 +1324,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
@@ -1353,16 +1350,13 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1375,46 +1369,46 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1429,7 +1423,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">

</xml_diff>